<commit_message>
Some changes to automatown and dtu
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/Automatown/cards.Datafile.xlsx
+++ b/CardFormatter/Data/Automatown/cards.Datafile.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="automa" sheetId="2" r:id="rId1"/>
-    <sheet name="Cards.Datafile" sheetId="4" r:id="rId2"/>
+    <sheet name="stations" sheetId="5" r:id="rId2"/>
+    <sheet name="goals" sheetId="6" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="212">
   <si>
     <t>image</t>
   </si>
@@ -295,18 +296,6 @@
     <t>{upgrade}x2, {collect}2{scrap.1}</t>
   </si>
   <si>
-    <t>{shooty}{handy}{tricky}</t>
-  </si>
-  <si>
-    <t>{handy}{tricky}</t>
-  </si>
-  <si>
-    <t>{shooty}{tricky}</t>
-  </si>
-  <si>
-    <t>{shooty}{handy}</t>
-  </si>
-  <si>
     <t>foo</t>
   </si>
   <si>
@@ -340,7 +329,337 @@
     <t>{downgrade}x2, {collect}2{scrap.1}, and {upgrade}x2</t>
   </si>
   <si>
-    <t/>
+    <t>SampleStation.png</t>
+  </si>
+  <si>
+    <t>station</t>
+  </si>
+  <si>
+    <t>Scrap Heap</t>
+  </si>
+  <si>
+    <t>{collect}7{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}5{scrap.1}</t>
+  </si>
+  <si>
+    <t>Low Quality Controller Station</t>
+  </si>
+  <si>
+    <t>{collect}2{controller.2} and 1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}1{controller.2} and 2{scrap.1}</t>
+  </si>
+  <si>
+    <t>Low Quality Sensor Station</t>
+  </si>
+  <si>
+    <t>{collect}2{sensor.2} and 1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}1{sensor.2} and 2{scrap.1}</t>
+  </si>
+  <si>
+    <t>Low Quality Motor Station</t>
+  </si>
+  <si>
+    <t>{collect}2{motor.2} and 1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}1{motor.2} and 2{scrap.1}</t>
+  </si>
+  <si>
+    <t>Pulverizer</t>
+  </si>
+  <si>
+    <t>{L2},{-&gt;},{collect}10{scrap.1}</t>
+  </si>
+  <si>
+    <t>{L2},{-&gt;},{collect}8{scrap.1}</t>
+  </si>
+  <si>
+    <t>{L2},{-&gt;},{collect}6{scrap.1}</t>
+  </si>
+  <si>
+    <t>Controller Station</t>
+  </si>
+  <si>
+    <t>{collect}1{controller.3}</t>
+  </si>
+  <si>
+    <t>Sensor Station</t>
+  </si>
+  <si>
+    <t>{collect}1{sensor.3}</t>
+  </si>
+  <si>
+    <t>Motor Station</t>
+  </si>
+  <si>
+    <t>{collect}1{motor.3}</t>
+  </si>
+  <si>
+    <t>Salvage shop</t>
+  </si>
+  <si>
+    <t>{L2},{-&gt;},{collect}2{L3}</t>
+  </si>
+  <si>
+    <t>{L2},{-&gt;},{collect}1{L4}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{L2},{-&gt;},{collect}1{L3}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>Controller Assembler</t>
+  </si>
+  <si>
+    <t>{collect}1{controller.3}, {upgrade}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}1{controller.2}, {upgrade}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>Sensors Assembler</t>
+  </si>
+  <si>
+    <t>{collect}1{sensor.3}, {upgrade}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}1{sensor.2}, {upgrade}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>Motor Assembler</t>
+  </si>
+  <si>
+    <t>{collect}1{motor.3}, {upgrade}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>{collect}1{motor.2}, {upgrade}, {collect}1{scrap.1}</t>
+  </si>
+  <si>
+    <t>One-Eyed Sam's Black Market</t>
+  </si>
+  <si>
+    <t>7{scrap.1},{-&gt;},{collect}1{controller.4},{collect}1{sensor.4}</t>
+  </si>
+  <si>
+    <t>2{scrap.1},{-&gt;},{collect}1{motor.4}</t>
+  </si>
+  <si>
+    <t>6{scrap.1},{-&gt;},{collect}1{sensor.2},{collect}1{motor.2},{collect}1{controller.2}</t>
+  </si>
+  <si>
+    <t>Motor Exchanger</t>
+  </si>
+  <si>
+    <t>{motor.4},{-&gt;},{collect}2 matching {L4}</t>
+  </si>
+  <si>
+    <t>{motor.3},{-&gt;},{collect}2 matching {L3}</t>
+  </si>
+  <si>
+    <t>{motor.2},{-&gt;},{collect}2 matching {L2}]</t>
+  </si>
+  <si>
+    <t>Controller Exchanger</t>
+  </si>
+  <si>
+    <t>{controller.4},{-&gt;},{collect}2 matching {L4}</t>
+  </si>
+  <si>
+    <t>{controller.3},{-&gt;},{collect}2 matching {L3}</t>
+  </si>
+  <si>
+    <t>{controller.2},{-&gt;},{collect}2 matching {L2}</t>
+  </si>
+  <si>
+    <t>Sensors Exchanger</t>
+  </si>
+  <si>
+    <t>{sensor.4},{-&gt;},{collect}2 matching {L4}</t>
+  </si>
+  <si>
+    <t>{sensor.3},{-&gt;},{collect}2 matching {L3}</t>
+  </si>
+  <si>
+    <t>{sensor.2},{-&gt;},{collect}2 matching {L2}</t>
+  </si>
+  <si>
+    <t>Junk Fixer/Giver</t>
+  </si>
+  <si>
+    <t>{collect}3{scrap.1}, {upgrade}4x</t>
+  </si>
+  <si>
+    <t>{collect}2{scrap.1}, {upgrade}3x</t>
+  </si>
+  <si>
+    <t>{collect}1{scrap.1}, {upgrade}2x</t>
+  </si>
+  <si>
+    <t>Recycling Station</t>
+  </si>
+  <si>
+    <t>2{scrap.1},{-&gt;},{collect}3 matching {L2}</t>
+  </si>
+  <si>
+    <t>2{scrap.1},{-&gt;},{collect}1{L4}</t>
+  </si>
+  <si>
+    <t>2{scrap.1},{-&gt;},{collect}1{L3}</t>
+  </si>
+  <si>
+    <t>Upgrade Station</t>
+  </si>
+  <si>
+    <t>{upgrade}x7</t>
+  </si>
+  <si>
+    <t>{upgrade}x5</t>
+  </si>
+  <si>
+    <t>{upgrade}x3</t>
+  </si>
+  <si>
+    <t>Upgrade/Scrap Shop</t>
+  </si>
+  <si>
+    <t>{collect}4{scrap.1}, {upgrade}x3</t>
+  </si>
+  <si>
+    <t>{collect}3{scrap.1}, {upgrade}x2</t>
+  </si>
+  <si>
+    <t>{collect}2{scrap.1}, {upgrade}</t>
+  </si>
+  <si>
+    <t>Component Juggler</t>
+  </si>
+  <si>
+    <t>{collect}3{scrap.1}, {upgrade}x2, {swap}x2</t>
+  </si>
+  <si>
+    <t>{collect}2{scrap.1}, {upgrade}, {swap}x2</t>
+  </si>
+  <si>
+    <t>{collect}2{scrap.1}, {swap}</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>cost 3</t>
+  </si>
+  <si>
+    <t>cost 2</t>
+  </si>
+  <si>
+    <t>cost 1</t>
+  </si>
+  <si>
+    <t>ability 3</t>
+  </si>
+  <si>
+    <t>ability 2</t>
+  </si>
+  <si>
+    <t>ability 1</t>
+  </si>
+  <si>
+    <t>SampleGoal.png</t>
+  </si>
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>Commit Arson</t>
+  </si>
+  <si>
+    <t>Steal candy from a baby</t>
+  </si>
+  <si>
+    <t>Assassinate the Mayor</t>
+  </si>
+  <si>
+    <t>Steal someones pet dog</t>
+  </si>
+  <si>
+    <t>Destroy the police station</t>
+  </si>
+  <si>
+    <t>Rob a bank</t>
+  </si>
+  <si>
+    <t>Rob a convenience store</t>
+  </si>
+  <si>
+    <t>Impersonate a store clerk</t>
+  </si>
+  <si>
+    <t>Shoot up the city</t>
+  </si>
+  <si>
+    <t>Rob a jewelry store</t>
+  </si>
+  <si>
+    <t>Manipulate the police</t>
+  </si>
+  <si>
+    <t>Take over town hall</t>
+  </si>
+  <si>
+    <t>Vandalize the courthouse</t>
+  </si>
+  <si>
+    <t>Vandalize a monument</t>
+  </si>
+  <si>
+    <t>Rob a sporting goods store</t>
+  </si>
+  <si>
+    <t>Impersonate a police officer</t>
+  </si>
+  <si>
+    <t>Take a hostage</t>
+  </si>
+  <si>
+    <t>Take over the mafia</t>
+  </si>
+  <si>
+    <t>Blackmail a government official</t>
+  </si>
+  <si>
+    <t>Encourage kids to smoke</t>
+  </si>
+  <si>
+    <t>Destroy a teacher's reputation</t>
+  </si>
+  <si>
+    <t>Impersonate the mayor</t>
+  </si>
+  <si>
+    <t>Con a judge</t>
+  </si>
+  <si>
+    <t>Impersonate the chief of police</t>
+  </si>
+  <si>
+    <t>Replace school superintendant</t>
+  </si>
+  <si>
+    <t>Convert the Mayor to evil</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Shoot a police robo-officer</t>
   </si>
 </sst>
 </file>
@@ -942,22 +1261,26 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="foes"/>
       <sheetName val="parts"/>
+      <sheetName val="chassis"/>
       <sheetName val="technologies"/>
       <sheetName val="characers"/>
-      <sheetName val="foes"/>
+      <sheetName val="extras"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="2">
           <cell r="L2" t="str">
             <v/>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -976,7 +1299,7 @@
     <tableColumn id="4" name="type"/>
     <tableColumn id="5" name="title"/>
     <tableColumn id="6" name="Req1"/>
-    <tableColumn id="8" name="r1" dataDxfId="0" dataCellStyle="Calculation">
+    <tableColumn id="8" name="r1" dataDxfId="14" dataCellStyle="Calculation">
       <calculatedColumnFormula>[1]parts!$L$2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Req2"/>
@@ -987,35 +1310,79 @@
     <tableColumn id="14" name="r3"/>
     <tableColumn id="15" name="Req4"/>
     <tableColumn id="17" name="r4"/>
-    <tableColumn id="19" name="icon" dataDxfId="14" dataCellStyle="Calculation">
+    <tableColumn id="19" name="icon" dataDxfId="13" dataCellStyle="Calculation">
       <calculatedColumnFormula>IF(T2=14, "{shooty}{handy}{tricky}", IF(T2=12, "{handy}{tricky}", IF(T2=10, "{shooty}{tricky}", IF(T2=8, "{tricky}", IF(T2=6, "{shooty}{handy}", IF(T2=4, "{handy}", IF(T2=2, "{shooty}", "")))))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" name="workers"/>
     <tableColumn id="24" name="ability"/>
-    <tableColumn id="31" name="Relative Power Level" dataDxfId="13">
+    <tableColumn id="31" name="Relative Power Level" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Workers value" dataDxfId="12" totalsRowDxfId="6">
+    <tableColumn id="22" name="Workers value" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(O2="{1automa}", 1, IF(O2="{2automa}", 2, IF(O2="{3automa}", 3,0)))*3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="25" name="Ability Value" dataCellStyle="Input"/>
-    <tableColumn id="20" name="Icon Value" dataDxfId="11" totalsRowDxfId="5" dataCellStyle="Input"/>
+    <tableColumn id="20" name="Icon Value" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Input"/>
     <tableColumn id="18" name="total cost">
       <calculatedColumnFormula>V2+W2+X2+Y2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost Value 1" dataDxfId="10" totalsRowDxfId="4">
+    <tableColumn id="7" name="Cost Value 1" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", F2)), 1, IF(ISNUMBER(SEARCH("2", F2)), 3, IF(ISNUMBER(SEARCH("3", F2)), 5, IF(ISNUMBER(SEARCH("4", F2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Cost Value 2" dataDxfId="9" totalsRowDxfId="3">
+    <tableColumn id="10" name="Cost Value 2" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", H2)), 1, IF(ISNUMBER(SEARCH("2", H2)), 3, IF(ISNUMBER(SEARCH("3", H2)), 5, IF(ISNUMBER(SEARCH("4", H2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Cost Value 3" dataDxfId="8" totalsRowDxfId="2">
+    <tableColumn id="13" name="Cost Value 3" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", J2)), 1, IF(ISNUMBER(SEARCH("2", J2)), 3, IF(ISNUMBER(SEARCH("3", J2)), 5, IF(ISNUMBER(SEARCH("4", J2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Cost Value 4" dataDxfId="7" totalsRowDxfId="1">
+    <tableColumn id="16" name="Cost Value 4" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", L2)), 1, IF(ISNUMBER(SEARCH("2", L2)), 3, IF(ISNUMBER(SEARCH("3", L2)), 5, IF(ISNUMBER(SEARCH("4", L2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="32" name="foo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L22" totalsRowShown="0">
+  <autoFilter ref="A1:L22"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="image"/>
+    <tableColumn id="2" name="name"/>
+    <tableColumn id="3" name="orientation"/>
+    <tableColumn id="4" name="type"/>
+    <tableColumn id="5" name="number"/>
+    <tableColumn id="6" name="location"/>
+    <tableColumn id="7" name="cost 3"/>
+    <tableColumn id="8" name="cost 2"/>
+    <tableColumn id="9" name="cost 1"/>
+    <tableColumn id="10" name="ability 3"/>
+    <tableColumn id="11" name="ability 2"/>
+    <tableColumn id="12" name="ability 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N28" totalsRowShown="0">
+  <autoFilter ref="A1:N28"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="image"/>
+    <tableColumn id="2" name="name"/>
+    <tableColumn id="3" name="orientation"/>
+    <tableColumn id="4" name="type"/>
+    <tableColumn id="5" name="title"/>
+    <tableColumn id="6" name="Req1"/>
+    <tableColumn id="7" name="r1"/>
+    <tableColumn id="8" name="Value"/>
+    <tableColumn id="9" name="Req2"/>
+    <tableColumn id="10" name="r2"/>
+    <tableColumn id="11" name="Req3"/>
+    <tableColumn id="12" name="r3"/>
+    <tableColumn id="13" name="Req4"/>
+    <tableColumn id="14" name="r4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1286,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -1373,34 +1740,34 @@
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="Z1" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -2217,7 +2584,7 @@
         <v>19</v>
       </c>
       <c r="P11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="Q11">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4212,18 +4579,18 @@
         <v>26</v>
       </c>
       <c r="I34" s="3" t="str">
-        <f t="shared" ref="I34:I65" si="10">IF(ISBLANK(H34), "", "{cc}")</f>
+        <f t="shared" ref="I34:I61" si="10">IF(ISBLANK(H34), "", "{cc}")</f>
         <v>{cc}</v>
       </c>
       <c r="J34" t="s">
         <v>26</v>
       </c>
       <c r="K34" s="3" t="str">
-        <f t="shared" ref="K34:K65" si="11">IF(ISBLANK(J34), "", "{cc}")</f>
+        <f t="shared" ref="K34:K61" si="11">IF(ISBLANK(J34), "", "{cc}")</f>
         <v>{cc}</v>
       </c>
       <c r="M34" s="3" t="str">
-        <f t="shared" ref="M34:M65" si="12">IF(ISBLANK(L34), "", "{cc}")</f>
+        <f t="shared" ref="M34:M61" si="12">IF(ISBLANK(L34), "", "{cc}")</f>
         <v/>
       </c>
       <c r="N34" s="3" t="str">
@@ -4248,7 +4615,7 @@
         <v>0</v>
       </c>
       <c r="U34" s="3">
-        <f t="shared" ref="U34:U65" si="15">V34+W34+X34+Y34</f>
+        <f t="shared" ref="U34:U61" si="15">V34+W34+X34+Y34</f>
         <v>3</v>
       </c>
       <c r="V34" s="3">
@@ -6540,33 +6907,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="95.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6580,6 +6941,875 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>136</v>
+      </c>
+      <c r="K13" t="s">
+        <v>137</v>
+      </c>
+      <c r="L13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>139</v>
+      </c>
+      <c r="K14" t="s">
+        <v>140</v>
+      </c>
+      <c r="L14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K15" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>147</v>
+      </c>
+      <c r="K16" t="s">
+        <v>148</v>
+      </c>
+      <c r="L16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>151</v>
+      </c>
+      <c r="K17" t="s">
+        <v>152</v>
+      </c>
+      <c r="L17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" t="s">
+        <v>156</v>
+      </c>
+      <c r="L18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" t="s">
+        <v>160</v>
+      </c>
+      <c r="L19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>163</v>
+      </c>
+      <c r="K20" t="s">
+        <v>164</v>
+      </c>
+      <c r="L20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>167</v>
+      </c>
+      <c r="K21" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>170</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>171</v>
+      </c>
+      <c r="K22" t="s">
+        <v>172</v>
+      </c>
+      <c r="L22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -6589,2800 +7819,1051 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>22</v>
+      <c r="H3">
+        <v>2</v>
       </c>
       <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" t="s">
         <v>24</v>
-      </c>
-      <c r="O4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>22</v>
+      <c r="H5">
+        <v>3</v>
       </c>
       <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
       <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="M5" t="s">
-        <v>105</v>
-      </c>
-      <c r="N5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
-        <v>28</v>
+      <c r="H6">
+        <v>3</v>
       </c>
       <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
         <v>21</v>
       </c>
-      <c r="K6" t="s">
-        <v>105</v>
-      </c>
-      <c r="M6" t="s">
-        <v>105</v>
-      </c>
-      <c r="N6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" t="s">
-        <v>30</v>
+      <c r="H7">
+        <v>4</v>
       </c>
       <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
         <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="N7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
-      </c>
-      <c r="O7" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
       </c>
       <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
-        <v>30</v>
+      <c r="H8">
+        <v>4</v>
       </c>
       <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
         <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" t="s">
-        <v>105</v>
-      </c>
-      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" t="s">
         <v>27</v>
-      </c>
-      <c r="O8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
       </c>
-      <c r="H9" t="s">
-        <v>28</v>
+      <c r="H9">
+        <v>4</v>
       </c>
       <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" t="s">
-        <v>105</v>
-      </c>
-      <c r="N9" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" t="s">
-        <v>105</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="H10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
-      </c>
-      <c r="O10" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
       </c>
       <c r="G11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" t="s">
-        <v>28</v>
+      <c r="H11">
+        <v>5</v>
       </c>
       <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
         <v>21</v>
       </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
       <c r="K11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" t="s">
         <v>21</v>
       </c>
       <c r="M11" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="N11" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>193</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
-        <v>22</v>
+      <c r="H12">
+        <v>5</v>
       </c>
       <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
         <v>21</v>
       </c>
-      <c r="J12" t="s">
-        <v>23</v>
-      </c>
       <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
         <v>21</v>
       </c>
-      <c r="M12" t="s">
-        <v>105</v>
-      </c>
-      <c r="N12" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>194</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
         <v>21</v>
       </c>
-      <c r="H13" t="s">
-        <v>20</v>
+      <c r="H13">
+        <v>5</v>
       </c>
       <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" t="s">
-        <v>93</v>
-      </c>
-      <c r="O13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" t="s">
-        <v>22</v>
+      <c r="H14">
+        <v>6</v>
       </c>
       <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
         <v>21</v>
       </c>
-      <c r="J14" t="s">
-        <v>22</v>
-      </c>
       <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" t="s">
         <v>21</v>
       </c>
-      <c r="L14" t="s">
-        <v>23</v>
-      </c>
       <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
         <v>21</v>
       </c>
-      <c r="N14" t="s">
-        <v>93</v>
-      </c>
-      <c r="O14" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>196</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
         <v>21</v>
       </c>
-      <c r="H15" t="s">
-        <v>22</v>
+      <c r="H15">
+        <v>6</v>
       </c>
       <c r="I15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
         <v>21</v>
       </c>
-      <c r="J15" t="s">
-        <v>23</v>
-      </c>
       <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
         <v>21</v>
       </c>
-      <c r="L15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" t="s">
-        <v>93</v>
-      </c>
-      <c r="O15" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
       </c>
-      <c r="H16" t="s">
-        <v>20</v>
+      <c r="H16">
+        <v>6</v>
       </c>
       <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
         <v>21</v>
       </c>
-      <c r="J16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
         <v>21</v>
       </c>
-      <c r="H17" t="s">
-        <v>28</v>
+      <c r="H17">
+        <v>7</v>
       </c>
       <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
         <v>21</v>
       </c>
-      <c r="J17" t="s">
-        <v>22</v>
-      </c>
       <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
         <v>21</v>
       </c>
-      <c r="L17" t="s">
-        <v>23</v>
-      </c>
       <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
         <v>21</v>
       </c>
-      <c r="N17" t="s">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18" t="s">
         <v>39</v>
-      </c>
-      <c r="O17" t="s">
-        <v>19</v>
-      </c>
-      <c r="P17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" t="s">
-        <v>20</v>
       </c>
       <c r="G18" t="s">
         <v>21</v>
       </c>
-      <c r="H18" t="s">
-        <v>22</v>
+      <c r="H18">
+        <v>7</v>
       </c>
       <c r="I18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" t="s">
         <v>21</v>
       </c>
-      <c r="J18" t="s">
-        <v>30</v>
-      </c>
       <c r="K18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" t="s">
         <v>21</v>
       </c>
-      <c r="L18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" t="s">
-        <v>22</v>
+      <c r="H19">
+        <v>8</v>
       </c>
       <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="s">
         <v>21</v>
       </c>
-      <c r="J19" t="s">
-        <v>23</v>
-      </c>
       <c r="K19" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" t="s">
         <v>21</v>
       </c>
-      <c r="L19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
         <v>21</v>
       </c>
-      <c r="H20" t="s">
-        <v>22</v>
+      <c r="H20">
+        <v>8</v>
       </c>
       <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
         <v>21</v>
       </c>
-      <c r="J20" t="s">
-        <v>23</v>
-      </c>
       <c r="K20" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" t="s">
         <v>21</v>
       </c>
       <c r="M20" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="N20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" t="s">
-        <v>19</v>
-      </c>
-      <c r="P20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
         <v>21</v>
       </c>
-      <c r="H21" t="s">
-        <v>22</v>
+      <c r="H21">
+        <v>8</v>
       </c>
       <c r="I21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" t="s">
         <v>21</v>
       </c>
-      <c r="J21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" t="s">
-        <v>92</v>
-      </c>
-      <c r="O21" t="s">
-        <v>19</v>
-      </c>
-      <c r="P21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
       </c>
-      <c r="H22" t="s">
-        <v>45</v>
+      <c r="H22">
+        <v>9</v>
       </c>
       <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" t="s">
-        <v>23</v>
-      </c>
       <c r="K22" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" t="s">
         <v>21</v>
       </c>
-      <c r="L22" t="s">
-        <v>26</v>
-      </c>
       <c r="M22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" t="s">
         <v>21</v>
       </c>
-      <c r="N22" t="s">
-        <v>92</v>
-      </c>
-      <c r="O22" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>204</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
         <v>21</v>
       </c>
-      <c r="H23" t="s">
-        <v>28</v>
+      <c r="H23">
+        <v>10</v>
       </c>
       <c r="I23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" t="s">
         <v>21</v>
       </c>
-      <c r="J23" t="s">
-        <v>43</v>
-      </c>
       <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" t="s">
         <v>21</v>
       </c>
-      <c r="L23" t="s">
-        <v>26</v>
-      </c>
       <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
         <v>21</v>
       </c>
-      <c r="N23" t="s">
-        <v>92</v>
-      </c>
-      <c r="O23" t="s">
-        <v>19</v>
-      </c>
-      <c r="P23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>205</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
         <v>21</v>
       </c>
-      <c r="H24" t="s">
-        <v>28</v>
+      <c r="H24">
+        <v>12</v>
       </c>
       <c r="I24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" t="s">
         <v>21</v>
       </c>
-      <c r="J24" t="s">
-        <v>30</v>
-      </c>
       <c r="K24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" t="s">
         <v>21</v>
       </c>
-      <c r="L24" t="s">
-        <v>26</v>
-      </c>
       <c r="M24" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" t="s">
         <v>21</v>
       </c>
-      <c r="N24" t="s">
-        <v>93</v>
-      </c>
-      <c r="O24" t="s">
-        <v>47</v>
-      </c>
-      <c r="P24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>206</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
       </c>
-      <c r="H25" t="s">
-        <v>45</v>
+      <c r="H25">
+        <v>12</v>
       </c>
       <c r="I25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" t="s">
         <v>21</v>
       </c>
-      <c r="J25" t="s">
-        <v>43</v>
-      </c>
       <c r="K25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" t="s">
         <v>21</v>
       </c>
-      <c r="M25" t="s">
-        <v>105</v>
-      </c>
-      <c r="N25" t="s">
-        <v>93</v>
-      </c>
-      <c r="O25" t="s">
-        <v>48</v>
-      </c>
-      <c r="P25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>207</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
       </c>
-      <c r="H26" t="s">
-        <v>45</v>
+      <c r="H26">
+        <v>13</v>
       </c>
       <c r="I26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" t="s">
         <v>21</v>
       </c>
-      <c r="J26" t="s">
-        <v>43</v>
-      </c>
       <c r="K26" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" t="s">
         <v>21</v>
       </c>
-      <c r="L26" t="s">
-        <v>26</v>
-      </c>
       <c r="M26" t="s">
+        <v>24</v>
+      </c>
+      <c r="N26" t="s">
         <v>21</v>
       </c>
-      <c r="N26" t="s">
-        <v>91</v>
-      </c>
-      <c r="O26" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>208</v>
       </c>
       <c r="F27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
       </c>
-      <c r="H27" t="s">
-        <v>45</v>
+      <c r="H27">
+        <v>14</v>
       </c>
       <c r="I27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" t="s">
         <v>21</v>
       </c>
-      <c r="J27" t="s">
-        <v>43</v>
-      </c>
       <c r="K27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" t="s">
         <v>21</v>
       </c>
       <c r="M27" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="N27" t="s">
-        <v>90</v>
-      </c>
-      <c r="O27" t="s">
-        <v>19</v>
-      </c>
-      <c r="P27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>209</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
       </c>
-      <c r="H28" t="s">
-        <v>45</v>
+      <c r="H28">
+        <v>16</v>
       </c>
       <c r="I28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" t="s">
         <v>21</v>
       </c>
-      <c r="J28" t="s">
-        <v>43</v>
-      </c>
       <c r="K28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" t="s">
         <v>21</v>
       </c>
       <c r="M28" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="N28" t="s">
-        <v>91</v>
-      </c>
-      <c r="O28" t="s">
-        <v>19</v>
-      </c>
-      <c r="P28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" t="s">
-        <v>41</v>
-      </c>
-      <c r="G29" t="s">
         <v>21</v>
-      </c>
-      <c r="H29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" t="s">
-        <v>45</v>
-      </c>
-      <c r="K29" t="s">
-        <v>21</v>
-      </c>
-      <c r="L29" t="s">
-        <v>43</v>
-      </c>
-      <c r="M29" t="s">
-        <v>21</v>
-      </c>
-      <c r="N29" t="s">
-        <v>90</v>
-      </c>
-      <c r="O29" t="s">
-        <v>19</v>
-      </c>
-      <c r="P29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" t="s">
-        <v>45</v>
-      </c>
-      <c r="I30" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" t="s">
-        <v>21</v>
-      </c>
-      <c r="L30" t="s">
-        <v>43</v>
-      </c>
-      <c r="M30" t="s">
-        <v>21</v>
-      </c>
-      <c r="N30" t="s">
-        <v>90</v>
-      </c>
-      <c r="O30" t="s">
-        <v>19</v>
-      </c>
-      <c r="P30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" t="s">
-        <v>43</v>
-      </c>
-      <c r="K31" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" t="s">
-        <v>23</v>
-      </c>
-      <c r="M31" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" t="s">
-        <v>90</v>
-      </c>
-      <c r="O31" t="s">
-        <v>19</v>
-      </c>
-      <c r="P31" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" t="s">
-        <v>51</v>
-      </c>
-      <c r="F32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32" t="s">
-        <v>105</v>
-      </c>
-      <c r="N32" t="s">
-        <v>105</v>
-      </c>
-      <c r="O32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F33" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" t="s">
-        <v>21</v>
-      </c>
-      <c r="M33" t="s">
-        <v>105</v>
-      </c>
-      <c r="N33" t="s">
-        <v>105</v>
-      </c>
-      <c r="O33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" t="s">
-        <v>105</v>
-      </c>
-      <c r="N34" t="s">
-        <v>105</v>
-      </c>
-      <c r="O34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" t="s">
-        <v>51</v>
-      </c>
-      <c r="F35" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" t="s">
-        <v>26</v>
-      </c>
-      <c r="K35" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35" t="s">
-        <v>105</v>
-      </c>
-      <c r="N35" t="s">
-        <v>105</v>
-      </c>
-      <c r="O35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36">
-        <v>35</v>
-      </c>
-      <c r="C36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" t="s">
-        <v>26</v>
-      </c>
-      <c r="G36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" t="s">
-        <v>26</v>
-      </c>
-      <c r="I36" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" t="s">
-        <v>26</v>
-      </c>
-      <c r="K36" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" t="s">
-        <v>105</v>
-      </c>
-      <c r="N36" t="s">
-        <v>105</v>
-      </c>
-      <c r="O36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" t="s">
-        <v>26</v>
-      </c>
-      <c r="I37" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" t="s">
-        <v>26</v>
-      </c>
-      <c r="K37" t="s">
-        <v>21</v>
-      </c>
-      <c r="M37" t="s">
-        <v>105</v>
-      </c>
-      <c r="N37" t="s">
-        <v>105</v>
-      </c>
-      <c r="O37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38">
-        <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38" t="s">
-        <v>26</v>
-      </c>
-      <c r="I38" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" t="s">
-        <v>26</v>
-      </c>
-      <c r="K38" t="s">
-        <v>21</v>
-      </c>
-      <c r="M38" t="s">
-        <v>105</v>
-      </c>
-      <c r="N38" t="s">
-        <v>105</v>
-      </c>
-      <c r="O38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" t="s">
-        <v>26</v>
-      </c>
-      <c r="G39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" t="s">
-        <v>26</v>
-      </c>
-      <c r="I39" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" t="s">
-        <v>26</v>
-      </c>
-      <c r="K39" t="s">
-        <v>21</v>
-      </c>
-      <c r="M39" t="s">
-        <v>105</v>
-      </c>
-      <c r="N39" t="s">
-        <v>105</v>
-      </c>
-      <c r="O39" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" t="s">
-        <v>26</v>
-      </c>
-      <c r="I40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" t="s">
-        <v>26</v>
-      </c>
-      <c r="K40" t="s">
-        <v>21</v>
-      </c>
-      <c r="M40" t="s">
-        <v>105</v>
-      </c>
-      <c r="N40" t="s">
-        <v>105</v>
-      </c>
-      <c r="O40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I41" t="s">
-        <v>21</v>
-      </c>
-      <c r="J41" t="s">
-        <v>26</v>
-      </c>
-      <c r="K41" t="s">
-        <v>21</v>
-      </c>
-      <c r="M41" t="s">
-        <v>105</v>
-      </c>
-      <c r="N41" t="s">
-        <v>105</v>
-      </c>
-      <c r="O41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" t="s">
-        <v>26</v>
-      </c>
-      <c r="I42" t="s">
-        <v>21</v>
-      </c>
-      <c r="J42" t="s">
-        <v>26</v>
-      </c>
-      <c r="K42" t="s">
-        <v>21</v>
-      </c>
-      <c r="M42" t="s">
-        <v>105</v>
-      </c>
-      <c r="N42" t="s">
-        <v>105</v>
-      </c>
-      <c r="O42" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" t="s">
-        <v>51</v>
-      </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-      <c r="G43" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" t="s">
-        <v>26</v>
-      </c>
-      <c r="I43" t="s">
-        <v>21</v>
-      </c>
-      <c r="J43" t="s">
-        <v>26</v>
-      </c>
-      <c r="K43" t="s">
-        <v>21</v>
-      </c>
-      <c r="M43" t="s">
-        <v>105</v>
-      </c>
-      <c r="N43" t="s">
-        <v>105</v>
-      </c>
-      <c r="O43" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44">
-        <v>43</v>
-      </c>
-      <c r="C44" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" t="s">
-        <v>51</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G44" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" t="s">
-        <v>26</v>
-      </c>
-      <c r="I44" t="s">
-        <v>21</v>
-      </c>
-      <c r="J44" t="s">
-        <v>26</v>
-      </c>
-      <c r="K44" t="s">
-        <v>21</v>
-      </c>
-      <c r="M44" t="s">
-        <v>105</v>
-      </c>
-      <c r="N44" t="s">
-        <v>105</v>
-      </c>
-      <c r="O44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45">
-        <v>44</v>
-      </c>
-      <c r="C45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" t="s">
-        <v>51</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-      <c r="G45" t="s">
-        <v>21</v>
-      </c>
-      <c r="H45" t="s">
-        <v>26</v>
-      </c>
-      <c r="I45" t="s">
-        <v>21</v>
-      </c>
-      <c r="J45" t="s">
-        <v>26</v>
-      </c>
-      <c r="K45" t="s">
-        <v>21</v>
-      </c>
-      <c r="M45" t="s">
-        <v>105</v>
-      </c>
-      <c r="N45" t="s">
-        <v>105</v>
-      </c>
-      <c r="O45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46">
-        <v>45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-      <c r="G46" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" t="s">
-        <v>26</v>
-      </c>
-      <c r="I46" t="s">
-        <v>21</v>
-      </c>
-      <c r="J46" t="s">
-        <v>26</v>
-      </c>
-      <c r="K46" t="s">
-        <v>21</v>
-      </c>
-      <c r="M46" t="s">
-        <v>105</v>
-      </c>
-      <c r="N46" t="s">
-        <v>105</v>
-      </c>
-      <c r="O46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47">
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" t="s">
-        <v>51</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-      <c r="G47" t="s">
-        <v>21</v>
-      </c>
-      <c r="H47" t="s">
-        <v>26</v>
-      </c>
-      <c r="I47" t="s">
-        <v>21</v>
-      </c>
-      <c r="J47" t="s">
-        <v>26</v>
-      </c>
-      <c r="K47" t="s">
-        <v>21</v>
-      </c>
-      <c r="M47" t="s">
-        <v>105</v>
-      </c>
-      <c r="N47" t="s">
-        <v>105</v>
-      </c>
-      <c r="O47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" t="s">
-        <v>51</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-      <c r="G48" t="s">
-        <v>21</v>
-      </c>
-      <c r="H48" t="s">
-        <v>26</v>
-      </c>
-      <c r="I48" t="s">
-        <v>21</v>
-      </c>
-      <c r="J48" t="s">
-        <v>26</v>
-      </c>
-      <c r="K48" t="s">
-        <v>21</v>
-      </c>
-      <c r="M48" t="s">
-        <v>105</v>
-      </c>
-      <c r="N48" t="s">
-        <v>105</v>
-      </c>
-      <c r="O48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" t="s">
-        <v>51</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
-      </c>
-      <c r="G49" t="s">
-        <v>21</v>
-      </c>
-      <c r="H49" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" t="s">
-        <v>21</v>
-      </c>
-      <c r="J49" t="s">
-        <v>26</v>
-      </c>
-      <c r="K49" t="s">
-        <v>21</v>
-      </c>
-      <c r="M49" t="s">
-        <v>105</v>
-      </c>
-      <c r="N49" t="s">
-        <v>105</v>
-      </c>
-      <c r="O49" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50">
-        <v>49</v>
-      </c>
-      <c r="C50" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-      <c r="G50" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" t="s">
-        <v>21</v>
-      </c>
-      <c r="J50" t="s">
-        <v>26</v>
-      </c>
-      <c r="K50" t="s">
-        <v>21</v>
-      </c>
-      <c r="M50" t="s">
-        <v>105</v>
-      </c>
-      <c r="N50" t="s">
-        <v>105</v>
-      </c>
-      <c r="O50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51">
-        <v>50</v>
-      </c>
-      <c r="C51" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" t="s">
-        <v>21</v>
-      </c>
-      <c r="H51" t="s">
-        <v>26</v>
-      </c>
-      <c r="I51" t="s">
-        <v>21</v>
-      </c>
-      <c r="J51" t="s">
-        <v>26</v>
-      </c>
-      <c r="K51" t="s">
-        <v>21</v>
-      </c>
-      <c r="M51" t="s">
-        <v>105</v>
-      </c>
-      <c r="N51" t="s">
-        <v>105</v>
-      </c>
-      <c r="O51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52">
-        <v>51</v>
-      </c>
-      <c r="C52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52" t="s">
-        <v>26</v>
-      </c>
-      <c r="G52" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" t="s">
-        <v>26</v>
-      </c>
-      <c r="I52" t="s">
-        <v>21</v>
-      </c>
-      <c r="J52" t="s">
-        <v>26</v>
-      </c>
-      <c r="K52" t="s">
-        <v>21</v>
-      </c>
-      <c r="M52" t="s">
-        <v>105</v>
-      </c>
-      <c r="N52" t="s">
-        <v>105</v>
-      </c>
-      <c r="O52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" t="s">
-        <v>51</v>
-      </c>
-      <c r="F53" t="s">
-        <v>26</v>
-      </c>
-      <c r="G53" t="s">
-        <v>21</v>
-      </c>
-      <c r="H53" t="s">
-        <v>26</v>
-      </c>
-      <c r="I53" t="s">
-        <v>21</v>
-      </c>
-      <c r="J53" t="s">
-        <v>26</v>
-      </c>
-      <c r="K53" t="s">
-        <v>21</v>
-      </c>
-      <c r="M53" t="s">
-        <v>105</v>
-      </c>
-      <c r="N53" t="s">
-        <v>105</v>
-      </c>
-      <c r="O53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54">
-        <v>53</v>
-      </c>
-      <c r="C54" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" t="s">
-        <v>51</v>
-      </c>
-      <c r="F54" t="s">
-        <v>26</v>
-      </c>
-      <c r="G54" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" t="s">
-        <v>26</v>
-      </c>
-      <c r="I54" t="s">
-        <v>21</v>
-      </c>
-      <c r="J54" t="s">
-        <v>26</v>
-      </c>
-      <c r="K54" t="s">
-        <v>21</v>
-      </c>
-      <c r="M54" t="s">
-        <v>105</v>
-      </c>
-      <c r="N54" t="s">
-        <v>105</v>
-      </c>
-      <c r="O54" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55">
-        <v>54</v>
-      </c>
-      <c r="C55" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" t="s">
-        <v>26</v>
-      </c>
-      <c r="G55" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" t="s">
-        <v>26</v>
-      </c>
-      <c r="I55" t="s">
-        <v>21</v>
-      </c>
-      <c r="J55" t="s">
-        <v>26</v>
-      </c>
-      <c r="K55" t="s">
-        <v>21</v>
-      </c>
-      <c r="M55" t="s">
-        <v>105</v>
-      </c>
-      <c r="N55" t="s">
-        <v>105</v>
-      </c>
-      <c r="O55" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56">
-        <v>55</v>
-      </c>
-      <c r="C56" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" t="s">
-        <v>51</v>
-      </c>
-      <c r="F56" t="s">
-        <v>26</v>
-      </c>
-      <c r="G56" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" t="s">
-        <v>26</v>
-      </c>
-      <c r="I56" t="s">
-        <v>21</v>
-      </c>
-      <c r="J56" t="s">
-        <v>26</v>
-      </c>
-      <c r="K56" t="s">
-        <v>21</v>
-      </c>
-      <c r="M56" t="s">
-        <v>105</v>
-      </c>
-      <c r="N56" t="s">
-        <v>105</v>
-      </c>
-      <c r="O56" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57">
-        <v>56</v>
-      </c>
-      <c r="C57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" t="s">
-        <v>51</v>
-      </c>
-      <c r="F57" t="s">
-        <v>26</v>
-      </c>
-      <c r="G57" t="s">
-        <v>21</v>
-      </c>
-      <c r="H57" t="s">
-        <v>26</v>
-      </c>
-      <c r="I57" t="s">
-        <v>21</v>
-      </c>
-      <c r="J57" t="s">
-        <v>26</v>
-      </c>
-      <c r="K57" t="s">
-        <v>21</v>
-      </c>
-      <c r="M57" t="s">
-        <v>105</v>
-      </c>
-      <c r="N57" t="s">
-        <v>105</v>
-      </c>
-      <c r="O57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58">
-        <v>57</v>
-      </c>
-      <c r="C58" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" t="s">
-        <v>51</v>
-      </c>
-      <c r="F58" t="s">
-        <v>26</v>
-      </c>
-      <c r="G58" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" t="s">
-        <v>26</v>
-      </c>
-      <c r="I58" t="s">
-        <v>21</v>
-      </c>
-      <c r="J58" t="s">
-        <v>26</v>
-      </c>
-      <c r="K58" t="s">
-        <v>21</v>
-      </c>
-      <c r="M58" t="s">
-        <v>105</v>
-      </c>
-      <c r="N58" t="s">
-        <v>105</v>
-      </c>
-      <c r="O58" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B59">
-        <v>58</v>
-      </c>
-      <c r="C59" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" t="s">
-        <v>18</v>
-      </c>
-      <c r="E59" t="s">
-        <v>51</v>
-      </c>
-      <c r="F59" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" t="s">
-        <v>26</v>
-      </c>
-      <c r="I59" t="s">
-        <v>21</v>
-      </c>
-      <c r="J59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K59" t="s">
-        <v>21</v>
-      </c>
-      <c r="M59" t="s">
-        <v>105</v>
-      </c>
-      <c r="N59" t="s">
-        <v>105</v>
-      </c>
-      <c r="O59" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>16</v>
-      </c>
-      <c r="B60">
-        <v>59</v>
-      </c>
-      <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" t="s">
-        <v>51</v>
-      </c>
-      <c r="F60" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60" t="s">
-        <v>26</v>
-      </c>
-      <c r="I60" t="s">
-        <v>21</v>
-      </c>
-      <c r="J60" t="s">
-        <v>26</v>
-      </c>
-      <c r="K60" t="s">
-        <v>21</v>
-      </c>
-      <c r="M60" t="s">
-        <v>105</v>
-      </c>
-      <c r="N60" t="s">
-        <v>105</v>
-      </c>
-      <c r="O60" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61">
-        <v>60</v>
-      </c>
-      <c r="C61" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" t="s">
-        <v>26</v>
-      </c>
-      <c r="G61" t="s">
-        <v>21</v>
-      </c>
-      <c r="H61" t="s">
-        <v>26</v>
-      </c>
-      <c r="I61" t="s">
-        <v>21</v>
-      </c>
-      <c r="J61" t="s">
-        <v>26</v>
-      </c>
-      <c r="K61" t="s">
-        <v>21</v>
-      </c>
-      <c r="M61" t="s">
-        <v>105</v>
-      </c>
-      <c r="N61" t="s">
-        <v>105</v>
-      </c>
-      <c r="O61" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lots of unchecked in work
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/Automatown/cards.Datafile.xlsx
+++ b/CardFormatter/Data/Automatown/cards.Datafile.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mike\CardGenerator\CardFormatter\Data\Automatown\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E497ED10-5F6D-454C-B341-9D98FEEB31F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="automa" sheetId="2" r:id="rId1"/>
     <sheet name="stations" sheetId="5" r:id="rId2"/>
     <sheet name="goals" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="385">
   <si>
     <t>image</t>
   </si>
@@ -242,9 +254,6 @@
     <t>{L2}{-&gt;}{collect}2x{controller.2}</t>
   </si>
   <si>
-    <t>{L3}{scrap.1}{-&gt;}{collect}2 matching {L3}</t>
-  </si>
-  <si>
     <t>{L2}{-&gt;}{collect}2x{sensor.2}</t>
   </si>
   <si>
@@ -503,9 +512,6 @@
     <t>Candybaby Daycare</t>
   </si>
   <si>
-    <t>Hugh's Highrise</t>
-  </si>
-  <si>
     <t>Totally not a Mafia Hangout</t>
   </si>
   <si>
@@ -530,12 +536,6 @@
     <t>The Nearly Dead Society</t>
   </si>
   <si>
-    <t>Barkley's dog kennel</t>
-  </si>
-  <si>
-    <t>Teen Rockstar's Mansion</t>
-  </si>
-  <si>
     <t>Denita's Fashion Emporium</t>
   </si>
   <si>
@@ -545,18 +545,9 @@
     <t>Ling's Bowling Alley</t>
   </si>
   <si>
-    <t>Nail Saloon</t>
-  </si>
-  <si>
     <t>The Pie-War Monument</t>
   </si>
   <si>
-    <t>Jim's sporting goods</t>
-  </si>
-  <si>
-    <t>The DMV</t>
-  </si>
-  <si>
     <t>Arcadia's Arcade</t>
   </si>
   <si>
@@ -566,12 +557,6 @@
     <t>River City Pool Hall</t>
   </si>
   <si>
-    <t>Johnny Cochran's Law Office</t>
-  </si>
-  <si>
-    <t>City Sanitation Office</t>
-  </si>
-  <si>
     <t>Uncle Moneypenny's Bank</t>
   </si>
   <si>
@@ -608,9 +593,6 @@
     <t>{motor.3}{-&gt;}{collect}2 matching {L3}</t>
   </si>
   <si>
-    <t>{motor.2}{-&gt;}{collect}2 matching {L2}]</t>
-  </si>
-  <si>
     <t>{controller.4}{-&gt;}{collect}2 matching {L4}</t>
   </si>
   <si>
@@ -644,27 +626,12 @@
     <t>Upgrade Scrap Shop</t>
   </si>
   <si>
-    <t>The For-Real Town Hall</t>
-  </si>
-  <si>
-    <t>The Mayor's house</t>
-  </si>
-  <si>
     <t>Rent-a-Cop Station</t>
   </si>
   <si>
     <t>The Casino for Dyscalculics</t>
   </si>
   <si>
-    <t>The Courthouse at 500 South</t>
-  </si>
-  <si>
-    <t>Chief of Police's house</t>
-  </si>
-  <si>
-    <t>Robo-cop Station</t>
-  </si>
-  <si>
     <t>Armando's Armored Truckstop</t>
   </si>
   <si>
@@ -731,9 +698,6 @@
     <t>{collect}{controller.2} AND {collect}2{scrap.1}</t>
   </si>
   <si>
-    <t>{collect}2{scrap.1}, {upgrade}x2 AND {swap}</t>
-  </si>
-  <si>
     <t>{collect}2{scrap.1}, {upgrade}x2</t>
   </si>
   <si>
@@ -1179,12 +1143,57 @@
   </si>
   <si>
     <t>{collect}{motor.2} AND {collect}4{scrap.1}</t>
+  </si>
+  <si>
+    <t>3{scrap.1}{-&gt;}{collect}2 matching {L3}</t>
+  </si>
+  <si>
+    <t>{collect}2{scrap.1}, {upgrade} AND {swap}</t>
+  </si>
+  <si>
+    <t>Mayor Quinby's house</t>
+  </si>
+  <si>
+    <t>Comissioner Gorden's House</t>
+  </si>
+  <si>
+    <t>Johnny Cochren's Law Office</t>
+  </si>
+  <si>
+    <t>The Gadgeteer's Headquarters</t>
+  </si>
+  <si>
+    <t>Brew Swayne's Mansion</t>
+  </si>
+  <si>
+    <t>The DMV of Sloths</t>
+  </si>
+  <si>
+    <t>Hugh's Huge Highrise</t>
+  </si>
+  <si>
+    <t>Judy's Courthouse</t>
+  </si>
+  <si>
+    <t>Silver Dollar Nail Saloon</t>
+  </si>
+  <si>
+    <t>Barkley's Dog Kennel</t>
+  </si>
+  <si>
+    <t>Goodies's Goodie shop</t>
+  </si>
+  <si>
+    <t>Mater's Truck Stop</t>
+  </si>
+  <si>
+    <t>Ye Olde Towne Halle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
@@ -1785,108 +1794,108 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z92" totalsRowCount="1" headerRowDxfId="16">
-  <autoFilter ref="A1:Z91"/>
-  <sortState ref="A2:Z91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Z92" totalsRowCount="1" headerRowDxfId="16">
+  <autoFilter ref="A1:Z91" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z91">
     <sortCondition descending="1" ref="U1:U91"/>
   </sortState>
   <tableColumns count="26">
-    <tableColumn id="1" name="image"/>
-    <tableColumn id="2" name="name" dataDxfId="15"/>
-    <tableColumn id="3" name="orientation"/>
-    <tableColumn id="4" name="type"/>
-    <tableColumn id="5" name="title"/>
-    <tableColumn id="6" name="Req1"/>
-    <tableColumn id="8" name="r1" dataDxfId="14" dataCellStyle="Calculation">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="image"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="orientation"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="title"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Req1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="r1" dataDxfId="14" dataCellStyle="Calculation">
       <calculatedColumnFormula>IF(ISBLANK(F2), "", "{cc}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Req2"/>
-    <tableColumn id="11" name="r2">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Req2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="r2">
       <calculatedColumnFormula>IF(ISBLANK(H2), "", "{cc}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Req3"/>
-    <tableColumn id="14" name="r3"/>
-    <tableColumn id="15" name="Req4"/>
-    <tableColumn id="17" name="r4"/>
-    <tableColumn id="19" name="icon" dataDxfId="13" dataCellStyle="Calculation">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Req3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="r3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Req4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="r4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="icon" dataDxfId="13" dataCellStyle="Calculation">
       <calculatedColumnFormula>IF(T2=14, "{shooty}{handy}{tricky}", IF(T2=12, "{handy}{tricky}", IF(T2=10, "{shooty}{tricky}", IF(T2=8, "{tricky}", IF(T2=6, "{shooty}{handy}", IF(T2=4, "{handy}", IF(T2=2, "{shooty}", "")))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="workers"/>
-    <tableColumn id="24" name="ability"/>
-    <tableColumn id="31" name="Relative Power Level" dataDxfId="12">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="workers"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ability"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Relative Power Level" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Workers value" dataDxfId="11" totalsRowDxfId="5">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Workers value" dataDxfId="11" totalsRowDxfId="5">
       <calculatedColumnFormula>IF(O2="{1automa}", 1, IF(O2="{2automa}", 2, IF(O2="{3automa}", 3,0)))*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Ability Value" dataCellStyle="Input"/>
-    <tableColumn id="20" name="Icon Value" dataDxfId="10" totalsRowDxfId="4" dataCellStyle="Input"/>
-    <tableColumn id="18" name="total cost">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Ability Value" dataCellStyle="Input"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Icon Value" dataDxfId="10" totalsRowDxfId="4" dataCellStyle="Input"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="total cost">
       <calculatedColumnFormula>V2+W2+X2+Y2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost Value 1" dataDxfId="9" totalsRowDxfId="3">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost Value 1" dataDxfId="9" totalsRowDxfId="3">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", F2)), 1, IF(ISNUMBER(SEARCH("2", F2)), 3, IF(ISNUMBER(SEARCH("3", F2)), 5, IF(ISNUMBER(SEARCH("4", F2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Cost Value 2" dataDxfId="8" totalsRowDxfId="2">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cost Value 2" dataDxfId="8" totalsRowDxfId="2">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", H2)), 1, IF(ISNUMBER(SEARCH("2", H2)), 3, IF(ISNUMBER(SEARCH("3", H2)), 5, IF(ISNUMBER(SEARCH("4", H2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Cost Value 3" dataDxfId="7" totalsRowDxfId="1">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Cost Value 3" dataDxfId="7" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", J2)), 1, IF(ISNUMBER(SEARCH("2", J2)), 3, IF(ISNUMBER(SEARCH("3", J2)), 5, IF(ISNUMBER(SEARCH("4", J2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Cost Value 4" dataDxfId="6" totalsRowDxfId="0">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Cost Value 4" dataDxfId="6" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("1", L2)), 1, IF(ISNUMBER(SEARCH("2", L2)), 3, IF(ISNUMBER(SEARCH("3", L2)), 5, IF(ISNUMBER(SEARCH("4", L2)), 7, 0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="foo"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="foo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L22" totalsRowShown="0">
-  <autoFilter ref="A1:L22"/>
-  <sortState ref="A2:L22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:L22" totalsRowShown="0">
+  <autoFilter ref="A1:L22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L22">
     <sortCondition ref="E1:E22"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="image"/>
-    <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="orientation"/>
-    <tableColumn id="4" name="type"/>
-    <tableColumn id="5" name="number"/>
-    <tableColumn id="6" name="location"/>
-    <tableColumn id="7" name="cost 3"/>
-    <tableColumn id="8" name="cost 2"/>
-    <tableColumn id="9" name="cost 1"/>
-    <tableColumn id="10" name="ability 3"/>
-    <tableColumn id="11" name="ability 2"/>
-    <tableColumn id="12" name="ability 1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="image"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="orientation"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="number"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="location"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="cost 3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="cost 2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="cost 1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ability 3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="ability 2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="ability 1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N37" totalsRowShown="0">
-  <autoFilter ref="A1:N37"/>
-  <sortState ref="A2:U35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:N37" totalsRowShown="0">
+  <autoFilter ref="A1:N37" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U35">
     <sortCondition ref="N1:N37"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="image"/>
-    <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="orientation"/>
-    <tableColumn id="4" name="type"/>
-    <tableColumn id="5" name="title"/>
-    <tableColumn id="6" name="Req1"/>
-    <tableColumn id="7" name="r1"/>
-    <tableColumn id="9" name="Req2"/>
-    <tableColumn id="10" name="r2"/>
-    <tableColumn id="11" name="Req3"/>
-    <tableColumn id="12" name="r3"/>
-    <tableColumn id="13" name="Req4"/>
-    <tableColumn id="14" name="r4"/>
-    <tableColumn id="8" name="Value"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="image"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="orientation"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="title"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Req1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="r1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Req2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="r2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Req3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="r3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Req4"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="r4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2154,12 +2163,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2244,34 +2253,34 @@
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="Z1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -2279,7 +2288,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -2326,7 +2335,7 @@
         <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q2">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -2368,7 +2377,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -2415,7 +2424,7 @@
         <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q3">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -2457,7 +2466,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -2504,7 +2513,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q4">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -2546,7 +2555,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -2635,7 +2644,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -2644,7 +2653,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
@@ -2682,7 +2691,7 @@
         <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="Q6">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -2724,7 +2733,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -2733,7 +2742,7 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -2771,7 +2780,7 @@
         <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="Q7">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -2813,7 +2822,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -2822,7 +2831,7 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F8" t="s">
         <v>25</v>
@@ -2860,7 +2869,7 @@
         <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="Q8">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -2902,7 +2911,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -2988,7 +2997,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -3074,7 +3083,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -3160,7 +3169,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -3207,7 +3216,7 @@
         <v>19</v>
       </c>
       <c r="P12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q12">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -3249,7 +3258,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -3296,7 +3305,7 @@
         <v>47</v>
       </c>
       <c r="P13" t="s">
-        <v>73</v>
+        <v>370</v>
       </c>
       <c r="Q13">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -3338,7 +3347,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -3385,7 +3394,7 @@
         <v>19</v>
       </c>
       <c r="P14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q14">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -3427,7 +3436,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -3516,7 +3525,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -3563,7 +3572,7 @@
         <v>19</v>
       </c>
       <c r="P16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q16">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -3605,7 +3614,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -3652,7 +3661,7 @@
         <v>19</v>
       </c>
       <c r="P17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q17">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -3694,7 +3703,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -3741,7 +3750,7 @@
         <v>19</v>
       </c>
       <c r="P18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q18">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -3783,7 +3792,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -3792,7 +3801,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
@@ -3863,7 +3872,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -3872,7 +3881,7 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
@@ -3946,7 +3955,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -3955,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="F21" t="s">
         <v>45</v>
@@ -4029,7 +4038,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -4073,7 +4082,7 @@
         <v>19</v>
       </c>
       <c r="P22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q22">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4115,7 +4124,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -4159,7 +4168,7 @@
         <v>19</v>
       </c>
       <c r="P23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q23">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4201,7 +4210,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -4245,7 +4254,7 @@
         <v>19</v>
       </c>
       <c r="P24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q24">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4287,7 +4296,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -4376,7 +4385,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -4465,7 +4474,7 @@
         <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -4554,7 +4563,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -4643,7 +4652,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -4684,7 +4693,7 @@
         <v>19</v>
       </c>
       <c r="P29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q29">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4726,7 +4735,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -4767,7 +4776,7 @@
         <v>19</v>
       </c>
       <c r="P30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q30">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4809,7 +4818,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -4850,7 +4859,7 @@
         <v>19</v>
       </c>
       <c r="P31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q31">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4892,7 +4901,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -4901,7 +4910,7 @@
         <v>18</v>
       </c>
       <c r="E32" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="F32" t="s">
         <v>41</v>
@@ -4933,7 +4942,7 @@
         <v>19</v>
       </c>
       <c r="P32" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="Q32">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -4975,7 +4984,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
@@ -4984,7 +4993,7 @@
         <v>18</v>
       </c>
       <c r="E33" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="F33" t="s">
         <v>41</v>
@@ -5016,7 +5025,7 @@
         <v>19</v>
       </c>
       <c r="P33" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="Q33">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5058,7 +5067,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
@@ -5067,7 +5076,7 @@
         <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F34" t="s">
         <v>45</v>
@@ -5099,7 +5108,7 @@
         <v>19</v>
       </c>
       <c r="P34" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="Q34">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5141,7 +5150,7 @@
         <v>16</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -5150,7 +5159,7 @@
         <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
@@ -5182,7 +5191,7 @@
         <v>19</v>
       </c>
       <c r="P35" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="Q35">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5224,7 +5233,7 @@
         <v>16</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
@@ -5233,7 +5242,7 @@
         <v>18</v>
       </c>
       <c r="E36" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
@@ -5265,7 +5274,7 @@
         <v>19</v>
       </c>
       <c r="P36" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="Q36">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5307,7 +5316,7 @@
         <v>16</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
@@ -5316,7 +5325,7 @@
         <v>18</v>
       </c>
       <c r="E37" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="F37" t="s">
         <v>22</v>
@@ -5348,7 +5357,7 @@
         <v>19</v>
       </c>
       <c r="P37" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="Q37">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5390,7 +5399,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
@@ -5434,7 +5443,7 @@
         <v>19</v>
       </c>
       <c r="P38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q38">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5476,7 +5485,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -5520,7 +5529,7 @@
         <v>19</v>
       </c>
       <c r="P39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q39">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5562,7 +5571,7 @@
         <v>16</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -5606,7 +5615,7 @@
         <v>19</v>
       </c>
       <c r="P40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q40">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5648,7 +5657,7 @@
         <v>16</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
@@ -5692,7 +5701,7 @@
         <v>19</v>
       </c>
       <c r="P41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q41">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5734,7 +5743,7 @@
         <v>16</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
@@ -5778,7 +5787,7 @@
         <v>19</v>
       </c>
       <c r="P42" t="s">
-        <v>236</v>
+        <v>371</v>
       </c>
       <c r="Q42">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5820,7 +5829,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -5864,7 +5873,7 @@
         <v>19</v>
       </c>
       <c r="P43" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="Q43">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5906,7 +5915,7 @@
         <v>16</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -5915,7 +5924,7 @@
         <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
@@ -5950,7 +5959,7 @@
         <v>19</v>
       </c>
       <c r="P44" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="Q44">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -5992,7 +6001,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -6001,7 +6010,7 @@
         <v>18</v>
       </c>
       <c r="E45" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
@@ -6036,7 +6045,7 @@
         <v>19</v>
       </c>
       <c r="P45" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="Q45">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -6078,7 +6087,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -6087,7 +6096,7 @@
         <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="F46" t="s">
         <v>26</v>
@@ -6122,7 +6131,7 @@
         <v>19</v>
       </c>
       <c r="P46" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="Q46">
         <f>Table1[[#This Row],[Workers value]]+Table1[[#This Row],[Ability Value]]+Table1[[#This Row],[Icon Value]]-Table1[[#This Row],[total cost]]</f>
@@ -6164,7 +6173,7 @@
         <v>16</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -6247,7 +6256,7 @@
         <v>16</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
@@ -6330,7 +6339,7 @@
         <v>16</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
@@ -6413,7 +6422,7 @@
         <v>16</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
@@ -6496,7 +6505,7 @@
         <v>16</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -6579,7 +6588,7 @@
         <v>16</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
@@ -6662,7 +6671,7 @@
         <v>16</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
@@ -6745,7 +6754,7 @@
         <v>16</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
@@ -6828,7 +6837,7 @@
         <v>16</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
@@ -6911,7 +6920,7 @@
         <v>16</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -6994,7 +7003,7 @@
         <v>16</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C57" t="s">
         <v>17</v>
@@ -7077,7 +7086,7 @@
         <v>16</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -7160,7 +7169,7 @@
         <v>16</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
@@ -7243,7 +7252,7 @@
         <v>16</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
@@ -7326,7 +7335,7 @@
         <v>16</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
@@ -7409,7 +7418,7 @@
         <v>16</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
@@ -7492,7 +7501,7 @@
         <v>16</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C63" t="s">
         <v>17</v>
@@ -7575,7 +7584,7 @@
         <v>16</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
@@ -7658,7 +7667,7 @@
         <v>16</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
@@ -7741,7 +7750,7 @@
         <v>16</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -7824,7 +7833,7 @@
         <v>16</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -7907,7 +7916,7 @@
         <v>16</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -7990,7 +7999,7 @@
         <v>16</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="C69" t="s">
         <v>17</v>
@@ -8073,7 +8082,7 @@
         <v>16</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
@@ -8156,7 +8165,7 @@
         <v>16</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="C71" t="s">
         <v>17</v>
@@ -8239,7 +8248,7 @@
         <v>16</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="C72" t="s">
         <v>17</v>
@@ -8322,7 +8331,7 @@
         <v>16</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="C73" t="s">
         <v>17</v>
@@ -8405,7 +8414,7 @@
         <v>16</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="C74" t="s">
         <v>17</v>
@@ -8488,7 +8497,7 @@
         <v>16</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="C75" t="s">
         <v>17</v>
@@ -8571,7 +8580,7 @@
         <v>16</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="C76" t="s">
         <v>17</v>
@@ -8654,7 +8663,7 @@
         <v>16</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="C77" t="s">
         <v>17</v>
@@ -8737,7 +8746,7 @@
         <v>16</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="C78" t="s">
         <v>17</v>
@@ -8820,7 +8829,7 @@
         <v>16</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="C79" t="s">
         <v>17</v>
@@ -8903,7 +8912,7 @@
         <v>16</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="C80" t="s">
         <v>17</v>
@@ -8986,7 +8995,7 @@
         <v>16</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="C81" t="s">
         <v>17</v>
@@ -9069,7 +9078,7 @@
         <v>16</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="C82" t="s">
         <v>17</v>
@@ -9152,7 +9161,7 @@
         <v>16</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="C83" t="s">
         <v>17</v>
@@ -9235,7 +9244,7 @@
         <v>16</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C84" t="s">
         <v>17</v>
@@ -9318,7 +9327,7 @@
         <v>16</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C85" t="s">
         <v>17</v>
@@ -9401,7 +9410,7 @@
         <v>16</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="C86" t="s">
         <v>17</v>
@@ -9484,7 +9493,7 @@
         <v>16</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="C87" t="s">
         <v>17</v>
@@ -9567,7 +9576,7 @@
         <v>16</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="C88" t="s">
         <v>17</v>
@@ -9650,7 +9659,7 @@
         <v>16</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -9733,7 +9742,7 @@
         <v>16</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="C90" t="s">
         <v>17</v>
@@ -9816,7 +9825,7 @@
         <v>16</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="C91" t="s">
         <v>17</v>
@@ -9948,11 +9957,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9983,48 +9992,48 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" t="s">
         <v>147</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>148</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>149</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>150</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>151</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>152</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>153</v>
-      </c>
-      <c r="L1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
@@ -10036,33 +10045,33 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="K2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="L2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>100</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
         <v>48</v>
@@ -10074,10 +10083,10 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
         <v>105</v>
-      </c>
-      <c r="K3" t="s">
-        <v>106</v>
       </c>
       <c r="L3" t="s">
         <v>35</v>
@@ -10085,22 +10094,22 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>99</v>
       </c>
-      <c r="B4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>100</v>
-      </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
         <v>48</v>
@@ -10112,10 +10121,10 @@
         <v>19</v>
       </c>
       <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" t="s">
         <v>108</v>
-      </c>
-      <c r="K4" t="s">
-        <v>109</v>
       </c>
       <c r="L4" t="s">
         <v>37</v>
@@ -10123,22 +10132,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" t="s">
         <v>48</v>
@@ -10150,10 +10159,10 @@
         <v>19</v>
       </c>
       <c r="J5" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" t="s">
         <v>111</v>
-      </c>
-      <c r="K5" t="s">
-        <v>112</v>
       </c>
       <c r="L5" t="s">
         <v>38</v>
@@ -10161,22 +10170,22 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>100</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
         <v>48</v>
@@ -10188,10 +10197,10 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" t="s">
         <v>102</v>
-      </c>
-      <c r="K6" t="s">
-        <v>103</v>
       </c>
       <c r="L6" t="s">
         <v>52</v>
@@ -10199,22 +10208,22 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>100</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" t="s">
         <v>48</v>
@@ -10226,10 +10235,10 @@
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L7" t="s">
         <v>35</v>
@@ -10237,22 +10246,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>100</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
         <v>48</v>
@@ -10264,10 +10273,10 @@
         <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L8" t="s">
         <v>37</v>
@@ -10275,22 +10284,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>99</v>
-      </c>
-      <c r="B9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>100</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" t="s">
         <v>48</v>
@@ -10302,10 +10311,10 @@
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" t="s">
         <v>38</v>
@@ -10313,22 +10322,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>246</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>100</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G10" t="s">
         <v>48</v>
@@ -10340,33 +10349,33 @@
         <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="K10" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>99</v>
-      </c>
-      <c r="B11" t="s">
-        <v>247</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>100</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
         <v>48</v>
@@ -10378,10 +10387,10 @@
         <v>19</v>
       </c>
       <c r="J11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" t="s">
         <v>122</v>
-      </c>
-      <c r="K11" t="s">
-        <v>123</v>
       </c>
       <c r="L11" t="s">
         <v>35</v>
@@ -10389,22 +10398,22 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>99</v>
-      </c>
-      <c r="B12" t="s">
-        <v>248</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" t="s">
         <v>48</v>
@@ -10416,10 +10425,10 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" t="s">
         <v>125</v>
-      </c>
-      <c r="K12" t="s">
-        <v>126</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -10427,22 +10436,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
         <v>99</v>
-      </c>
-      <c r="B13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
       </c>
       <c r="E13">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
         <v>48</v>
@@ -10454,10 +10463,10 @@
         <v>19</v>
       </c>
       <c r="J13" t="s">
+        <v>127</v>
+      </c>
+      <c r="K13" t="s">
         <v>128</v>
-      </c>
-      <c r="K13" t="s">
-        <v>129</v>
       </c>
       <c r="L13" t="s">
         <v>38</v>
@@ -10465,22 +10474,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>99</v>
-      </c>
-      <c r="B14" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>100</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G14" t="s">
         <v>48</v>
@@ -10492,33 +10501,33 @@
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="K14" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="L14" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
         <v>99</v>
-      </c>
-      <c r="B15" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>100</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
@@ -10530,33 +10539,33 @@
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K15" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="L15" t="s">
-        <v>195</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
         <v>99</v>
-      </c>
-      <c r="B16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>100</v>
       </c>
       <c r="E16">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G16" t="s">
         <v>48</v>
@@ -10568,33 +10577,33 @@
         <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="K16" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="L16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>99</v>
-      </c>
-      <c r="B17" t="s">
-        <v>253</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>100</v>
       </c>
       <c r="E17">
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G17" t="s">
         <v>48</v>
@@ -10606,33 +10615,33 @@
         <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="K17" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
         <v>99</v>
       </c>
-      <c r="B18" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>100</v>
-      </c>
       <c r="E18">
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="G18" t="s">
         <v>48</v>
@@ -10644,33 +10653,33 @@
         <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="K18" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="L18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
         <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>255</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>100</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G19" t="s">
         <v>48</v>
@@ -10682,33 +10691,33 @@
         <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="K19" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="L19" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>240</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>99</v>
-      </c>
-      <c r="B20" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>100</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G20" t="s">
         <v>48</v>
@@ -10720,33 +10729,33 @@
         <v>19</v>
       </c>
       <c r="J20" t="s">
+        <v>136</v>
+      </c>
+      <c r="K20" t="s">
         <v>137</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>138</v>
-      </c>
-      <c r="L20" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>99</v>
-      </c>
-      <c r="B21" t="s">
-        <v>257</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>100</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="G21" t="s">
         <v>48</v>
@@ -10758,33 +10767,33 @@
         <v>19</v>
       </c>
       <c r="J21" t="s">
+        <v>139</v>
+      </c>
+      <c r="K21" t="s">
         <v>140</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>141</v>
-      </c>
-      <c r="L21" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
         <v>99</v>
-      </c>
-      <c r="B22" t="s">
-        <v>258</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" t="s">
-        <v>100</v>
       </c>
       <c r="E22">
         <v>21</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G22" t="s">
         <v>48</v>
@@ -10796,13 +10805,13 @@
         <v>19</v>
       </c>
       <c r="J22" t="s">
+        <v>143</v>
+      </c>
+      <c r="K22" t="s">
         <v>144</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>145</v>
-      </c>
-      <c r="L22" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -10815,11 +10824,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10881,24 +10890,24 @@
         <v>13</v>
       </c>
       <c r="N1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>155</v>
       </c>
-      <c r="B2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>156</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -10912,19 +10921,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>155</v>
       </c>
-      <c r="B3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>156</v>
-      </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
@@ -10938,19 +10947,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>155</v>
       </c>
-      <c r="B4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>156</v>
-      </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -10970,19 +10979,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>155</v>
       </c>
-      <c r="B5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>156</v>
-      </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>381</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
@@ -11002,19 +11011,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>155</v>
       </c>
-      <c r="B6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>156</v>
-      </c>
       <c r="E6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -11040,19 +11049,19 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>155</v>
       </c>
-      <c r="B7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>156</v>
-      </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -11072,19 +11081,19 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>155</v>
       </c>
-      <c r="B8" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>156</v>
-      </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
@@ -11110,19 +11119,19 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>155</v>
       </c>
-      <c r="B9" t="s">
-        <v>266</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>156</v>
-      </c>
       <c r="E9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -11154,19 +11163,19 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>155</v>
       </c>
-      <c r="B10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>156</v>
-      </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
@@ -11180,19 +11189,19 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>155</v>
       </c>
-      <c r="B11" t="s">
-        <v>268</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>156</v>
-      </c>
       <c r="E11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
@@ -11218,19 +11227,19 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>155</v>
       </c>
-      <c r="B12" t="s">
-        <v>269</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>156</v>
-      </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F12" t="s">
         <v>27</v>
@@ -11262,19 +11271,19 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
         <v>155</v>
       </c>
-      <c r="B13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>156</v>
-      </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>380</v>
       </c>
       <c r="F13" t="s">
         <v>39</v>
@@ -11294,19 +11303,19 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>155</v>
       </c>
-      <c r="B14" t="s">
-        <v>271</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>156</v>
-      </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
@@ -11332,19 +11341,19 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
         <v>155</v>
       </c>
-      <c r="B15" t="s">
-        <v>272</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>156</v>
-      </c>
       <c r="E15" t="s">
-        <v>211</v>
+        <v>379</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
@@ -11376,19 +11385,19 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
         <v>155</v>
       </c>
-      <c r="B16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>156</v>
-      </c>
       <c r="E16" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
@@ -11408,19 +11417,19 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>155</v>
       </c>
-      <c r="B17" t="s">
-        <v>274</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>156</v>
-      </c>
       <c r="E17" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -11446,19 +11455,19 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
         <v>155</v>
       </c>
-      <c r="B18" t="s">
-        <v>275</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>156</v>
-      </c>
       <c r="E18" t="s">
-        <v>176</v>
+        <v>383</v>
       </c>
       <c r="F18" t="s">
         <v>27</v>
@@ -11490,19 +11499,19 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
         <v>155</v>
       </c>
-      <c r="B19" t="s">
-        <v>276</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>156</v>
-      </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>378</v>
       </c>
       <c r="F19" t="s">
         <v>39</v>
@@ -11528,19 +11537,19 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
+        <v>261</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>155</v>
       </c>
-      <c r="B20" t="s">
-        <v>277</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>156</v>
-      </c>
       <c r="E20" t="s">
-        <v>177</v>
+        <v>377</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
@@ -11572,19 +11581,19 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="s">
+        <v>262</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>155</v>
       </c>
-      <c r="B21" t="s">
-        <v>278</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>156</v>
-      </c>
       <c r="E21" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F21" t="s">
         <v>27</v>
@@ -11616,19 +11625,19 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
         <v>155</v>
       </c>
-      <c r="B22" t="s">
-        <v>279</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" t="s">
-        <v>156</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
@@ -11654,19 +11663,19 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
         <v>155</v>
       </c>
-      <c r="B23" t="s">
-        <v>280</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" t="s">
-        <v>156</v>
-      </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F23" t="s">
         <v>39</v>
@@ -11698,19 +11707,19 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s">
+        <v>265</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
         <v>155</v>
       </c>
-      <c r="B24" t="s">
-        <v>281</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>156</v>
-      </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>382</v>
       </c>
       <c r="F24" t="s">
         <v>39</v>
@@ -11730,19 +11739,19 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>266</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
         <v>155</v>
       </c>
-      <c r="B25" t="s">
-        <v>282</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" t="s">
-        <v>156</v>
-      </c>
       <c r="E25" t="s">
-        <v>212</v>
+        <v>373</v>
       </c>
       <c r="F25" t="s">
         <v>39</v>
@@ -11774,19 +11783,19 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
         <v>155</v>
       </c>
-      <c r="B26" t="s">
-        <v>283</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" t="s">
-        <v>156</v>
-      </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F26" t="s">
         <v>39</v>
@@ -11812,19 +11821,19 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
         <v>155</v>
       </c>
-      <c r="B27" t="s">
-        <v>284</v>
-      </c>
-      <c r="C27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" t="s">
-        <v>156</v>
-      </c>
       <c r="E27" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F27" t="s">
         <v>39</v>
@@ -11856,19 +11865,19 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
         <v>155</v>
       </c>
-      <c r="B28" t="s">
-        <v>285</v>
-      </c>
-      <c r="C28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" t="s">
-        <v>156</v>
-      </c>
       <c r="E28" t="s">
-        <v>181</v>
+        <v>374</v>
       </c>
       <c r="F28" t="s">
         <v>39</v>
@@ -11894,19 +11903,19 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>270</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
         <v>155</v>
       </c>
-      <c r="B29" t="s">
-        <v>286</v>
-      </c>
-      <c r="C29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" t="s">
-        <v>156</v>
-      </c>
       <c r="E29" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F29" t="s">
         <v>39</v>
@@ -11938,19 +11947,19 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
         <v>155</v>
       </c>
-      <c r="B30" t="s">
-        <v>287</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" t="s">
-        <v>156</v>
-      </c>
       <c r="E30" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F30" t="s">
         <v>39</v>
@@ -11982,19 +11991,19 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
         <v>155</v>
       </c>
-      <c r="B31" t="s">
-        <v>288</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" t="s">
-        <v>156</v>
-      </c>
       <c r="E31" t="s">
-        <v>208</v>
+        <v>372</v>
       </c>
       <c r="F31" t="s">
         <v>39</v>
@@ -12026,19 +12035,19 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
         <v>155</v>
       </c>
-      <c r="B32" t="s">
-        <v>289</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
-        <v>156</v>
-      </c>
       <c r="E32" t="s">
-        <v>170</v>
+        <v>376</v>
       </c>
       <c r="F32" t="s">
         <v>39</v>
@@ -12064,19 +12073,19 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" t="s">
+        <v>274</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
         <v>155</v>
       </c>
-      <c r="B33" t="s">
-        <v>290</v>
-      </c>
-      <c r="C33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" t="s">
-        <v>156</v>
-      </c>
       <c r="E33" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F33" t="s">
         <v>39</v>
@@ -12108,19 +12117,19 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
         <v>155</v>
       </c>
-      <c r="B34" t="s">
-        <v>291</v>
-      </c>
-      <c r="C34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" t="s">
-        <v>156</v>
-      </c>
       <c r="E34" t="s">
-        <v>213</v>
+        <v>375</v>
       </c>
       <c r="F34" t="s">
         <v>39</v>
@@ -12152,19 +12161,19 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
         <v>155</v>
       </c>
-      <c r="B35" t="s">
-        <v>292</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" t="s">
-        <v>156</v>
-      </c>
       <c r="E35" t="s">
-        <v>207</v>
+        <v>384</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>

</xml_diff>